<commit_message>
feat: busca A* (falta definir algumas heurísticas)
</commit_message>
<xml_diff>
--- a/distancias_aereo.xlsx
+++ b/distancias_aereo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neves\Desktop\UTFPR\IA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neves\PycharmProjects\trabIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7266B5B9-BBDB-4D8E-A986-6EFD3389420D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2CF4EE-290D-45FD-865C-585F5F299455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{668EB7BF-DB79-4251-A746-DEE8BBFEB7C5}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
   <si>
     <t>Origem</t>
   </si>
@@ -70,12 +70,6 @@
     <t>Teresina</t>
   </si>
   <si>
-    <t>B. Horizonte</t>
-  </si>
-  <si>
-    <t>C. Grande</t>
-  </si>
-  <si>
     <t>Aracajú</t>
   </si>
   <si>
@@ -116,7 +110,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,6 +241,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -593,8 +595,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -950,10 +953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D48B53B-215B-43AC-AFC9-ECE87D82461E}">
-  <dimension ref="A1:AB29"/>
+  <dimension ref="A1:AB31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X8" sqref="X8"/>
+      <selection activeCell="AA28" sqref="AA28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,10 +966,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -975,34 +978,34 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
       </c>
       <c r="J1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K1" t="s">
         <v>5</v>
       </c>
       <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
         <v>23</v>
       </c>
-      <c r="M1" t="s">
-        <v>25</v>
-      </c>
       <c r="N1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" t="s">
         <v>24</v>
-      </c>
-      <c r="O1" t="s">
-        <v>26</v>
       </c>
       <c r="P1" t="s">
         <v>6</v>
@@ -1032,21 +1035,21 @@
         <v>14</v>
       </c>
       <c r="Y1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Z1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="AA1" t="s">
         <v>15</v>
       </c>
       <c r="AB1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1088,54 +1091,54 @@
         <v>1967</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>2673</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>604</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>1235</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>2580</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>2946</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>398</v>
       </c>
       <c r="V2">
-        <v>0</v>
+        <v>3359</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <v>1482</v>
       </c>
       <c r="X2">
-        <v>0</v>
+        <v>277</v>
       </c>
       <c r="Y2">
-        <v>0</v>
+        <v>1226</v>
       </c>
       <c r="Z2">
-        <v>0</v>
+        <v>1731</v>
       </c>
       <c r="AA2">
-        <v>0</v>
+        <v>903</v>
       </c>
       <c r="AB2">
-        <v>0</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1641</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1218,13 +1221,13 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1248</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>2111</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1307,13 +1310,13 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>3022</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1432</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>3117</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1390,19 +1393,19 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1292</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1592</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>624</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>2496</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -1476,22 +1479,22 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>2155</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>2212</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1118</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>2667</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>878</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -1562,25 +1565,25 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>2121</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1778</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1372</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>2107</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>873</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>559</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1651,25 +1654,25 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>2061</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>2665</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>820</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>3370</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1081</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>780</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>1302</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -1734,31 +1737,31 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>2207</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>2904</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>973</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>3620</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1314</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1007</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1543</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>251</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1823,31 +1826,31 @@
         <v>5</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>815</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1133</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1893</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>2562</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1687</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>2547</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>2329</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>2670</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>2857</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -1906,37 +1909,37 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1461</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1693</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>666</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>2503</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>173</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>705</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>740</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>972</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>1215</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>1854</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -1992,40 +1995,40 @@
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>486</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1636</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1726</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>3067</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1716</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>2593</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>2495</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>2545</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>2693</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>555</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>1889</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -2078,43 +2081,43 @@
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1967</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>329</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>2349</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>1110</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>1791</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>2309</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>1822</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>2836</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>3082</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>1451</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>1868</v>
       </c>
       <c r="M14">
-        <v>0</v>
+        <v>1964</v>
       </c>
       <c r="N14">
         <v>0</v>
@@ -2164,46 +2167,46 @@
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1680</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1439</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>3089</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>1485</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>2352</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>2302</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>2259</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>2402</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>730</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>1656</v>
       </c>
       <c r="M15">
-        <v>0</v>
+        <v>299</v>
       </c>
       <c r="N15">
-        <v>0</v>
+        <v>2009</v>
       </c>
       <c r="O15">
         <v>0</v>
@@ -2253,46 +2256,46 @@
         <v>6</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>2673</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>1292</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>2556</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>661</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>1932</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>2013</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>1453</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>2734</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>2981</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>2383</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>1912</v>
       </c>
       <c r="M16">
-        <v>0</v>
+        <v>2819</v>
       </c>
       <c r="N16">
-        <v>0</v>
+        <v>1054</v>
       </c>
       <c r="O16">
-        <v>0</v>
+        <v>2778</v>
       </c>
       <c r="P16">
         <v>0</v>
@@ -2339,49 +2342,49 @@
         <v>7</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>604</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>1550</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1831</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>2983</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>1775</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>2654</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>2524</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>2645</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>2802</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>435</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>1948</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <v>151</v>
       </c>
       <c r="N17">
-        <v>0</v>
+        <v>1874</v>
       </c>
       <c r="O17">
-        <v>0</v>
+        <v>434</v>
       </c>
       <c r="P17">
-        <v>0</v>
+        <v>2765</v>
       </c>
       <c r="Q17">
         <v>0</v>
@@ -2425,52 +2428,52 @@
         <v>8</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>1235</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>973</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1178</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>1988</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>620</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>1320</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>1029</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>1693</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>1931</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>1300</v>
       </c>
       <c r="L18">
-        <v>0</v>
+        <v>724</v>
       </c>
       <c r="M18">
-        <v>0</v>
+        <v>1521</v>
       </c>
       <c r="N18">
-        <v>0</v>
+        <v>1177</v>
       </c>
       <c r="O18">
-        <v>0</v>
+        <v>1383</v>
       </c>
       <c r="P18">
-        <v>0</v>
+        <v>1509</v>
       </c>
       <c r="Q18">
-        <v>0</v>
+        <v>1527</v>
       </c>
       <c r="R18">
         <v>0</v>
@@ -2511,55 +2514,55 @@
         <v>9</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>2580</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>3188</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>1341</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>3785</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>1619</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>1119</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>1679</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>546</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>376</v>
       </c>
       <c r="K19">
-        <v>0</v>
+        <v>3213</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>1497</v>
       </c>
       <c r="M19">
-        <v>0</v>
+        <v>3066</v>
       </c>
       <c r="N19">
-        <v>0</v>
+        <v>3341</v>
       </c>
       <c r="O19">
-        <v>0</v>
+        <v>2775</v>
       </c>
       <c r="P19">
-        <v>0</v>
+        <v>3132</v>
       </c>
       <c r="Q19">
-        <v>0</v>
+        <v>3172</v>
       </c>
       <c r="R19">
-        <v>0</v>
+        <v>2222</v>
       </c>
       <c r="S19">
         <v>0</v>
@@ -2597,58 +2600,58 @@
         <v>10</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>2946</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>1886</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>2477</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>1335</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>1900</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>1634</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>1137</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>2412</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>2641</v>
       </c>
       <c r="K20">
-        <v>0</v>
+        <v>2855</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>1813</v>
       </c>
       <c r="M20">
-        <v>0</v>
+        <v>3200</v>
       </c>
       <c r="N20">
-        <v>0</v>
+        <v>1724</v>
       </c>
       <c r="O20">
-        <v>0</v>
+        <v>3090</v>
       </c>
       <c r="P20">
-        <v>0</v>
+        <v>761</v>
       </c>
       <c r="Q20">
-        <v>0</v>
+        <v>3179</v>
       </c>
       <c r="R20">
-        <v>0</v>
+        <v>1711</v>
       </c>
       <c r="S20">
-        <v>0</v>
+        <v>2706</v>
       </c>
       <c r="T20">
         <v>0</v>
@@ -2683,61 +2686,61 @@
         <v>11</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>398</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1676</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1639</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>3103</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>1657</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>2530</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>2452</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>2459</v>
       </c>
       <c r="J21">
-        <v>0</v>
+        <v>2603</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>629</v>
       </c>
       <c r="L21">
-        <v>0</v>
+        <v>1829</v>
       </c>
       <c r="M21">
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="N21">
-        <v>0</v>
+        <v>2005</v>
       </c>
       <c r="O21">
-        <v>0</v>
+        <v>202</v>
       </c>
       <c r="P21">
-        <v>0</v>
+        <v>2833</v>
       </c>
       <c r="Q21">
-        <v>0</v>
+        <v>253</v>
       </c>
       <c r="R21">
-        <v>0</v>
+        <v>1498</v>
       </c>
       <c r="S21">
-        <v>0</v>
+        <v>2977</v>
       </c>
       <c r="T21">
-        <v>0</v>
+        <v>3190</v>
       </c>
       <c r="U21">
         <v>0</v>
@@ -2769,64 +2772,64 @@
         <v>12</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>3359</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>2333</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>2786</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>1626</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>2246</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>1827</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>1414</v>
       </c>
       <c r="I22">
-        <v>0</v>
+        <v>2601</v>
       </c>
       <c r="J22">
-        <v>0</v>
+        <v>2809</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>3300</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>2138</v>
       </c>
       <c r="M22">
-        <v>0</v>
+        <v>3632</v>
       </c>
       <c r="N22">
-        <v>0</v>
+        <v>2159</v>
       </c>
       <c r="O22">
-        <v>0</v>
+        <v>3510</v>
       </c>
       <c r="P22">
-        <v>0</v>
+        <v>1149</v>
       </c>
       <c r="Q22">
-        <v>0</v>
+        <v>3616</v>
       </c>
       <c r="R22">
-        <v>0</v>
+        <v>2127</v>
       </c>
       <c r="S22">
-        <v>0</v>
+        <v>2814</v>
       </c>
       <c r="T22">
-        <v>0</v>
+        <v>449</v>
       </c>
       <c r="U22">
-        <v>0</v>
+        <v>3618</v>
       </c>
       <c r="V22">
         <v>0</v>
@@ -2855,67 +2858,67 @@
         <v>13</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>1482</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>2450</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>339</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>3428</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>933</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>1212</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>1575</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>675</v>
       </c>
       <c r="J23">
-        <v>0</v>
+        <v>748</v>
       </c>
       <c r="K23">
-        <v>0</v>
+        <v>2190</v>
       </c>
       <c r="L23">
-        <v>0</v>
+        <v>936</v>
       </c>
       <c r="M23">
-        <v>0</v>
+        <v>1968</v>
       </c>
       <c r="N23">
-        <v>0</v>
+        <v>2687</v>
       </c>
       <c r="O23">
-        <v>0</v>
+        <v>1671</v>
       </c>
       <c r="P23">
-        <v>0</v>
+        <v>2849</v>
       </c>
       <c r="Q23">
-        <v>0</v>
+        <v>2085</v>
       </c>
       <c r="R23">
-        <v>0</v>
+        <v>1512</v>
       </c>
       <c r="S23">
-        <v>0</v>
+        <v>1123</v>
       </c>
       <c r="T23">
-        <v>0</v>
+        <v>2707</v>
       </c>
       <c r="U23">
-        <v>0</v>
+        <v>1874</v>
       </c>
       <c r="V23">
-        <v>0</v>
+        <v>2982</v>
       </c>
       <c r="W23">
         <v>0</v>
@@ -2941,70 +2944,70 @@
         <v>14</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>277</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1687</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>964</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>3009</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>1060</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>1905</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>1915</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>1784</v>
       </c>
       <c r="J24">
-        <v>0</v>
+        <v>1930</v>
       </c>
       <c r="K24">
-        <v>0</v>
+        <v>1028</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>1225</v>
       </c>
       <c r="M24">
-        <v>0</v>
+        <v>763</v>
       </c>
       <c r="N24">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="O24">
-        <v>0</v>
+        <v>475</v>
       </c>
       <c r="P24">
-        <v>0</v>
+        <v>2605</v>
       </c>
       <c r="Q24">
-        <v>0</v>
+        <v>875</v>
       </c>
       <c r="R24">
-        <v>0</v>
+        <v>1114</v>
       </c>
       <c r="S24">
-        <v>0</v>
+        <v>2303</v>
       </c>
       <c r="T24">
-        <v>0</v>
+        <v>2808</v>
       </c>
       <c r="U24">
-        <v>0</v>
+        <v>675</v>
       </c>
       <c r="V24">
-        <v>0</v>
+        <v>3206</v>
       </c>
       <c r="W24">
-        <v>0</v>
+        <v>1209</v>
       </c>
       <c r="X24">
         <v>0</v>
@@ -3024,76 +3027,76 @@
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>1226</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>481</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>1932</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>1913</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>1524</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>2284</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>1942</v>
       </c>
       <c r="I25">
-        <v>0</v>
+        <v>2599</v>
       </c>
       <c r="J25">
-        <v>0</v>
+        <v>2821</v>
       </c>
       <c r="K25">
-        <v>0</v>
+        <v>652</v>
       </c>
       <c r="L25">
-        <v>0</v>
+        <v>1662</v>
       </c>
       <c r="M25">
-        <v>0</v>
+        <v>1162</v>
       </c>
       <c r="N25">
-        <v>0</v>
+        <v>803</v>
       </c>
       <c r="O25">
-        <v>0</v>
+        <v>1234</v>
       </c>
       <c r="P25">
-        <v>0</v>
+        <v>1746</v>
       </c>
       <c r="Q25">
-        <v>0</v>
+        <v>1071</v>
       </c>
       <c r="R25">
-        <v>0</v>
+        <v>964</v>
       </c>
       <c r="S25">
-        <v>0</v>
+        <v>3142</v>
       </c>
       <c r="T25">
-        <v>0</v>
+        <v>2274</v>
       </c>
       <c r="U25">
-        <v>0</v>
+        <v>1209</v>
       </c>
       <c r="V25">
-        <v>0</v>
+        <v>2726</v>
       </c>
       <c r="W25">
-        <v>0</v>
+        <v>2266</v>
       </c>
       <c r="X25">
-        <v>0</v>
+        <v>1323</v>
       </c>
       <c r="Y25">
         <v>0</v>
@@ -3110,79 +3113,79 @@
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>1731</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>2463</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>489</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>3300</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>873</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>894</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>1326</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>338</v>
       </c>
       <c r="J26">
-        <v>0</v>
+        <v>489</v>
       </c>
       <c r="K26">
-        <v>0</v>
+        <v>2368</v>
       </c>
       <c r="L26">
-        <v>0</v>
+        <v>810</v>
       </c>
       <c r="M26">
-        <v>0</v>
+        <v>2216</v>
       </c>
       <c r="N26">
-        <v>0</v>
+        <v>2664</v>
       </c>
       <c r="O26">
-        <v>0</v>
+        <v>1928</v>
       </c>
       <c r="P26">
-        <v>0</v>
+        <v>2689</v>
       </c>
       <c r="Q26">
-        <v>0</v>
+        <v>2320</v>
       </c>
       <c r="R26">
-        <v>0</v>
+        <v>1493</v>
       </c>
       <c r="S26">
-        <v>0</v>
+        <v>852</v>
       </c>
       <c r="T26">
-        <v>0</v>
+        <v>2463</v>
       </c>
       <c r="U26">
-        <v>0</v>
+        <v>2128</v>
       </c>
       <c r="V26">
-        <v>0</v>
+        <v>2704</v>
       </c>
       <c r="W26">
-        <v>0</v>
+        <v>357</v>
       </c>
       <c r="X26">
-        <v>0</v>
+        <v>1453</v>
       </c>
       <c r="Y26">
-        <v>0</v>
+        <v>2348</v>
       </c>
       <c r="Z26">
         <v>0</v>
@@ -3199,79 +3202,79 @@
         <v>15</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>903</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>1652</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>2169</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>1313</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>2132</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>1862</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>2362</v>
       </c>
       <c r="J27">
-        <v>0</v>
+        <v>2573</v>
       </c>
       <c r="K27">
-        <v>0</v>
+        <v>495</v>
       </c>
       <c r="L27">
-        <v>0</v>
+        <v>1467</v>
       </c>
       <c r="M27">
-        <v>0</v>
+        <v>905</v>
       </c>
       <c r="N27">
-        <v>0</v>
+        <v>1079</v>
       </c>
       <c r="O27">
-        <v>0</v>
+        <v>929</v>
       </c>
       <c r="P27">
-        <v>0</v>
+        <v>1921</v>
       </c>
       <c r="Q27">
-        <v>0</v>
+        <v>843</v>
       </c>
       <c r="R27">
-        <v>0</v>
+        <v>835</v>
       </c>
       <c r="S27">
-        <v>0</v>
+        <v>2909</v>
       </c>
       <c r="T27">
-        <v>0</v>
+        <v>2362</v>
       </c>
       <c r="U27">
-        <v>0</v>
+        <v>934</v>
       </c>
       <c r="V27">
-        <v>0</v>
+        <v>2806</v>
       </c>
       <c r="W27">
-        <v>0</v>
+        <v>1979</v>
       </c>
       <c r="X27">
-        <v>0</v>
+        <v>994</v>
       </c>
       <c r="Y27">
-        <v>0</v>
+        <v>329</v>
       </c>
       <c r="Z27">
-        <v>0</v>
+        <v>2091</v>
       </c>
       <c r="AA27">
         <v>0</v>
@@ -3282,175 +3285,92 @@
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>1102</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>2275</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>378</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>3394</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>947</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>1490</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>1745</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>1076</v>
       </c>
       <c r="J28">
-        <v>0</v>
+        <v>1160</v>
       </c>
       <c r="K28">
-        <v>0</v>
+        <v>1855</v>
       </c>
       <c r="L28">
-        <v>0</v>
+        <v>1022</v>
       </c>
       <c r="M28">
-        <v>0</v>
+        <v>1581</v>
       </c>
       <c r="N28">
-        <v>0</v>
+        <v>2545</v>
       </c>
       <c r="O28">
-        <v>0</v>
+        <v>1282</v>
       </c>
       <c r="P28">
-        <v>0</v>
+        <v>2865</v>
       </c>
       <c r="Q28">
-        <v>0</v>
+        <v>1706</v>
       </c>
       <c r="R28">
-        <v>0</v>
+        <v>1413</v>
       </c>
       <c r="S28">
-        <v>0</v>
+        <v>1536</v>
       </c>
       <c r="T28">
-        <v>0</v>
+        <v>2835</v>
       </c>
       <c r="U28">
-        <v>0</v>
+        <v>1483</v>
       </c>
       <c r="V28">
-        <v>0</v>
+        <v>3156</v>
       </c>
       <c r="W28">
-        <v>0</v>
+        <v>412</v>
       </c>
       <c r="X28">
-        <v>0</v>
+        <v>839</v>
       </c>
       <c r="Y28">
-        <v>0</v>
+        <v>2023</v>
       </c>
       <c r="Z28">
-        <v>0</v>
+        <v>741</v>
       </c>
       <c r="AA28">
-        <v>0</v>
+        <v>1713</v>
       </c>
       <c r="AB28">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>18</v>
-      </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-      <c r="M29">
-        <v>0</v>
-      </c>
-      <c r="N29">
-        <v>0</v>
-      </c>
-      <c r="O29">
-        <v>201</v>
-      </c>
-      <c r="P29">
-        <v>2673</v>
-      </c>
-      <c r="Q29">
-        <v>604</v>
-      </c>
-      <c r="R29">
-        <v>1235</v>
-      </c>
-      <c r="S29">
-        <v>2580</v>
-      </c>
-      <c r="T29">
-        <v>2946</v>
-      </c>
-      <c r="U29">
-        <v>398</v>
-      </c>
-      <c r="V29">
-        <v>3359</v>
-      </c>
-      <c r="W29">
-        <v>1482</v>
-      </c>
-      <c r="X29">
-        <v>277</v>
-      </c>
-      <c r="Y29">
-        <v>1226</v>
-      </c>
-      <c r="Z29">
-        <v>1731</v>
-      </c>
-      <c r="AA29">
-        <v>903</v>
-      </c>
-      <c r="AB29">
-        <v>1102</v>
-      </c>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I31" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>